<commit_message>
JCM007- Update Print template
</commit_message>
<xml_diff>
--- a/nts.uk/uk.hr/hr.file/nts.uk.file.hr.infra/src/main/resources/report/退職者登録一覧_Template.xlsx
+++ b/nts.uk/uk.hr/hr.file/nts.uk.file.hr.infra/src/main/resources/report/退職者登録一覧_Template.xlsx
@@ -199,10 +199,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44172,10 +44168,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A3:AJ3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Z1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="AJ12" sqref="AJ12"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="90" zoomScaleNormal="120" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -44230,8 +44229,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <pageMargins left="0.43307086614173229" right="0.23622047244094491" top="0.74803149606299213" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" fitToWidth="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.43307086614173201" right="0.23622047244094499" top="0.74803149606299202" bottom="0.55118110236220497" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup paperSize="9" scale="36" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L日通システム株式会社&amp;C&amp;"ＭＳ ゴシック,標準"&amp;16退職者登録一覧&amp;R&amp;D　&amp;T　
 page&amp;P</oddHeader>

</xml_diff>